<commit_message>
Stakeholder Analysis update Budget Summary Upload
</commit_message>
<xml_diff>
--- a/documentation/projman/Week 1 -3/Nacor Industries - Stakeholder Analysis.xlsx
+++ b/documentation/projman/Week 1 -3/Nacor Industries - Stakeholder Analysis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://asiapacificcollege.sharepoint.com/sites/PROJMANT3MI201MI203/Shared Documents/Group 04 Nacor Industries/Midterm Deliverables/Week 1 - 3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rthrm\Documents\APC_2022_2023_T3_PROJMAN_MI201_MI203_G04_Nacor_Industries\documentation\projman\Week 1 -3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="188" documentId="11_0A2E3C54391981D9B0DE0FD4B277FC0736D8502B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{594F9033-D9D5-4951-A269-150E9ACCBD26}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18FD844-2A8B-4951-8E2C-21B8B2714BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>Stakeholder Analysis</t>
   </si>
@@ -101,27 +101,6 @@
     <t>Not willing to provide feedback or communicate with the development team</t>
   </si>
   <si>
-    <t>Sir Hans Schuck</t>
-  </si>
-  <si>
-    <t>Project Consultant</t>
-  </si>
-  <si>
-    <t>Provide insights and suggestions regarding the UI/UX of the application and discuss possible pain points.</t>
-  </si>
-  <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>Give supporting feedback to the current progress, suggest improvements and additional details to the project, answer inquiries depending on their specialization</t>
-  </si>
-  <si>
-    <t>Miss Wednesday Gadon</t>
-  </si>
-  <si>
-    <t>Provide insights and suggestions regarding the documentation and representation of the application and discuss business opportunities.</t>
-  </si>
-  <si>
     <t>APC-ITRO</t>
   </si>
   <si>
@@ -140,9 +119,6 @@
     <t>Refusal to learn the new system</t>
   </si>
   <si>
-    <t>APC Students &amp; Faculty</t>
-  </si>
-  <si>
     <t>Asia Pacific College</t>
   </si>
   <si>
@@ -150,6 +126,9 @@
   </si>
   <si>
     <t>Refusal to use the new system</t>
+  </si>
+  <si>
+    <t>APC Students, Faculty &amp; Staff</t>
   </si>
 </sst>
 </file>
@@ -216,7 +195,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -226,48 +205,24 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -280,65 +235,53 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -623,10 +566,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -645,16 +588,16 @@
   <sheetData>
     <row r="1" spans="1:26" ht="27.75" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -703,28 +646,28 @@
     </row>
     <row r="3" spans="1:26" ht="53.25" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="8" t="s">
         <v>8</v>
       </c>
       <c r="J3" s="1"/>
@@ -747,26 +690,26 @@
     </row>
     <row r="4" spans="1:26" ht="93.75" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="19" t="s">
+      <c r="E4" s="10"/>
+      <c r="F4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="10" t="s">
         <v>15</v>
       </c>
       <c r="J4" s="1"/>
@@ -789,26 +732,26 @@
     </row>
     <row r="5" spans="1:26" ht="90.75" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11" t="s">
+      <c r="E5" s="17"/>
+      <c r="F5" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="15" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="17" t="s">
         <v>21</v>
       </c>
       <c r="J5" s="1"/>
@@ -831,27 +774,27 @@
     </row>
     <row r="6" spans="1:26" ht="60" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="15" t="s">
+      <c r="C6" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16" t="s">
+      <c r="D6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="E6" s="10"/>
+      <c r="F6" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="G6" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="16" t="s">
-        <v>21</v>
+      <c r="I6" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -871,29 +814,29 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7" spans="1:26" ht="74.25" customHeight="1">
+    <row r="7" spans="1:26" ht="60" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="8" t="s">
-        <v>27</v>
+      <c r="B7" s="16" t="s">
+        <v>31</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11" t="s">
+      <c r="C7" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>25</v>
+      <c r="D7" s="16" t="s">
+        <v>24</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="E7" s="17"/>
+      <c r="F7" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="11" t="s">
-        <v>21</v>
+      <c r="I7" s="17" t="s">
+        <v>30</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -913,30 +856,16 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" spans="1:26" ht="60" customHeight="1">
+    <row r="8" spans="1:26" ht="27" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>34</v>
-      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -955,30 +884,16 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" spans="1:26" ht="60" customHeight="1">
+    <row r="9" spans="1:26" ht="27" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>38</v>
-      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -999,8 +914,8 @@
     </row>
     <row r="10" spans="1:26" ht="27" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -1027,14 +942,14 @@
     </row>
     <row r="11" spans="1:26" ht="27" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -1055,14 +970,14 @@
     </row>
     <row r="12" spans="1:26" ht="27" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -1725,7 +1640,7 @@
       <c r="Y35" s="1"/>
       <c r="Z35" s="1"/>
     </row>
-    <row r="36" spans="1:26" ht="27" customHeight="1">
+    <row r="36" spans="1:26" ht="15.75" customHeight="1">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1753,7 +1668,7 @@
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
     </row>
-    <row r="37" spans="1:26" ht="27" customHeight="1">
+    <row r="37" spans="1:26" ht="15.75" customHeight="1">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -6765,62 +6680,8 @@
       <c r="Y215" s="1"/>
       <c r="Z215" s="1"/>
     </row>
-    <row r="216" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A216" s="1"/>
-      <c r="B216" s="1"/>
-      <c r="C216" s="1"/>
-      <c r="D216" s="1"/>
-      <c r="E216" s="1"/>
-      <c r="F216" s="1"/>
-      <c r="G216" s="1"/>
-      <c r="H216" s="1"/>
-      <c r="I216" s="1"/>
-      <c r="J216" s="1"/>
-      <c r="K216" s="1"/>
-      <c r="L216" s="1"/>
-      <c r="M216" s="1"/>
-      <c r="N216" s="1"/>
-      <c r="O216" s="1"/>
-      <c r="P216" s="1"/>
-      <c r="Q216" s="1"/>
-      <c r="R216" s="1"/>
-      <c r="S216" s="1"/>
-      <c r="T216" s="1"/>
-      <c r="U216" s="1"/>
-      <c r="V216" s="1"/>
-      <c r="W216" s="1"/>
-      <c r="X216" s="1"/>
-      <c r="Y216" s="1"/>
-      <c r="Z216" s="1"/>
-    </row>
-    <row r="217" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A217" s="1"/>
-      <c r="B217" s="1"/>
-      <c r="C217" s="1"/>
-      <c r="D217" s="1"/>
-      <c r="E217" s="1"/>
-      <c r="F217" s="1"/>
-      <c r="G217" s="1"/>
-      <c r="H217" s="1"/>
-      <c r="I217" s="1"/>
-      <c r="J217" s="1"/>
-      <c r="K217" s="1"/>
-      <c r="L217" s="1"/>
-      <c r="M217" s="1"/>
-      <c r="N217" s="1"/>
-      <c r="O217" s="1"/>
-      <c r="P217" s="1"/>
-      <c r="Q217" s="1"/>
-      <c r="R217" s="1"/>
-      <c r="S217" s="1"/>
-      <c r="T217" s="1"/>
-      <c r="U217" s="1"/>
-      <c r="V217" s="1"/>
-      <c r="W217" s="1"/>
-      <c r="X217" s="1"/>
-      <c r="Y217" s="1"/>
-      <c r="Z217" s="1"/>
-    </row>
+    <row r="216" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="217" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="218" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="219" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="220" spans="1:26" ht="15.75" customHeight="1"/>
@@ -7599,8 +7460,6 @@
     <row r="993" ht="15.75" customHeight="1"/>
     <row r="994" ht="15.75" customHeight="1"/>
     <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:I1"/>
@@ -7611,15 +7470,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010078E5C03F786D684AB79627F2BAF5AB3A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6753d19c26ced2570449d2cfe2fd38cd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="31aac78f-6ed8-4134-ac7e-47c186d487c3" xmlns:ns3="0d803109-e11b-45d4-a4e8-5bf0740163af" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="59531f12ec9f3761682ad3919ac9365f" ns2:_="" ns3:_="">
     <xsd:import namespace="31aac78f-6ed8-4134-ac7e-47c186d487c3"/>
@@ -7836,10 +7686,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CF9527F-EB29-4169-B7E6-78E929F64951}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2EAC03B-7253-4032-AE30-32F91736985A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="31aac78f-6ed8-4134-ac7e-47c186d487c3"/>
+    <ds:schemaRef ds:uri="0d803109-e11b-45d4-a4e8-5bf0740163af"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2EAC03B-7253-4032-AE30-32F91736985A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CF9527F-EB29-4169-B7E6-78E929F64951}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>